<commit_message>
Se activa un logs detallado de las inserciones y se verifica wu no se inserten dupicados
</commit_message>
<xml_diff>
--- a/mastertables/MasterTables.xlsx
+++ b/mastertables/MasterTables.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="18"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="18"/>
   </bookViews>
   <sheets>
     <sheet name="format" sheetId="1" state="visible" r:id="rId2"/>
@@ -25,8 +25,8 @@
     <sheet name="season" sheetId="15" state="visible" r:id="rId16"/>
     <sheet name="filter" sheetId="16" state="visible" r:id="rId17"/>
     <sheet name="gain" sheetId="17" state="visible" r:id="rId18"/>
-    <sheet name="project" sheetId="18" state="visible" r:id="rId19"/>
-    <sheet name="funding" sheetId="19" state="visible" r:id="rId20"/>
+    <sheet name="funding" sheetId="18" state="visible" r:id="rId19"/>
+    <sheet name="project" sheetId="19" state="visible" r:id="rId20"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -4111,16 +4111,16 @@
     <t xml:space="preserve">SISTEMIC</t>
   </si>
   <si>
+    <t xml:space="preserve">MINCIENCIAS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Universidad de Antioquia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ISAGEN-GHA</t>
+  </si>
+  <si>
     <t xml:space="preserve">CONSERVACIÓN BIOLÓGICA USANDO INTELIGENCIA ARTIFICIAL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MINCIENCIAS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Universidad de Antioquia</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ISAGEN-GHA</t>
   </si>
 </sst>
 </file>
@@ -4130,11 +4130,12 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -4155,6 +4156,12 @@
       <sz val="11"/>
       <name val="Cambria"/>
       <family val="1"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -4199,7 +4206,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -4212,33 +4219,34 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
 </styleSheet>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A2" activeCellId="1" sqref="B1:B3 A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.3418367346939"/>
-  </cols>
+  <sheetFormatPr defaultColWidth="11.35546875" defaultRowHeight="12" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
@@ -4253,7 +4261,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.789583333333333" right="0.789583333333333" top="1.01944444444444" bottom="1.01944444444444" header="0.789583333333333" footer="0.789583333333333"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPágina &amp;P</oddFooter>
@@ -4262,20 +4270,19 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:A4"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A6" activeCellId="1" sqref="B1:B3 A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12"/>
+  <sheetFormatPr defaultColWidth="11.35546875" defaultRowHeight="12" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.8112244897959"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="11.3418367346939"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="22.81"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4301,7 +4308,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.789583333333333" right="0.789583333333333" top="1.01944444444444" bottom="1.01944444444444" header="0.789583333333333" footer="0.789583333333333"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPágina &amp;P</oddFooter>
@@ -4310,20 +4317,17 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:A5"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D11" activeCellId="0" sqref="D11"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D11" activeCellId="1" sqref="B1:B3 D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.3418367346939"/>
-  </cols>
+  <sheetFormatPr defaultColWidth="11.35546875" defaultRowHeight="12" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
@@ -4353,7 +4357,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.789583333333333" right="0.789583333333333" top="1.01944444444444" bottom="1.01944444444444" header="0.789583333333333" footer="0.789583333333333"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPágina &amp;P</oddFooter>
@@ -4362,20 +4366,17 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="B1:B3 A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.3418367346939"/>
-  </cols>
+  <sheetFormatPr defaultColWidth="11.35546875" defaultRowHeight="12" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
@@ -4385,7 +4386,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.789583333333333" right="0.789583333333333" top="1.01944444444444" bottom="1.01944444444444" header="0.789583333333333" footer="0.789583333333333"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPágina &amp;P</oddFooter>
@@ -4394,20 +4395,17 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A2" activeCellId="1" sqref="B1:B3 A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.3418367346939"/>
-  </cols>
+  <sheetFormatPr defaultColWidth="11.35546875" defaultRowHeight="12" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
@@ -4422,7 +4420,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.789583333333333" right="0.789583333333333" top="1.01944444444444" bottom="1.01944444444444" header="0.789583333333333" footer="0.789583333333333"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPágina &amp;P</oddFooter>
@@ -4431,20 +4429,19 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:A9"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E21" activeCellId="0" sqref="E21"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E21" activeCellId="1" sqref="B1:B3 E21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12"/>
+  <sheetFormatPr defaultColWidth="11.35546875" defaultRowHeight="12" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.8214285714286"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="11.3418367346939"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.82"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4495,7 +4492,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.789583333333333" right="0.789583333333333" top="1.01944444444444" bottom="1.01944444444444" header="0.789583333333333" footer="0.789583333333333"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPágina &amp;P</oddFooter>
@@ -4504,20 +4501,17 @@
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:A5"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D20" activeCellId="0" sqref="D20"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D20" activeCellId="1" sqref="B1:B3 D20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.3418367346939"/>
-  </cols>
+  <sheetFormatPr defaultColWidth="11.35546875" defaultRowHeight="12" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
@@ -4547,7 +4541,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.789583333333333" right="0.789583333333333" top="1.01944444444444" bottom="1.01944444444444" header="0.789583333333333" footer="0.789583333333333"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPágina &amp;P</oddFooter>
@@ -4556,20 +4550,19 @@
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:A4"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="B1:B3 A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12"/>
+  <sheetFormatPr defaultColWidth="11.35546875" defaultRowHeight="12" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="25.2448979591837"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="11.3418367346939"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="25.24"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4595,7 +4588,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.789583333333333" right="0.789583333333333" top="1.01944444444444" bottom="1.01944444444444" header="0.789583333333333" footer="0.789583333333333"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPágina &amp;P</oddFooter>
@@ -4604,20 +4597,19 @@
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:A6"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D21" activeCellId="0" sqref="D21"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D21" activeCellId="1" sqref="B1:B3 D21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12"/>
+  <sheetFormatPr defaultColWidth="11.35546875" defaultRowHeight="12" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="29.4285714285714"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="11.3418367346939"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="29.43"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4653,7 +4645,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.789583333333333" right="0.789583333333333" top="1.01944444444444" bottom="1.01944444444444" header="0.789583333333333" footer="0.789583333333333"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPágina &amp;P</oddFooter>
@@ -4662,19 +4654,19 @@
 </file>
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:A3"/>
+  <dimension ref="A1:A5"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A3" activeCellId="1" sqref="B1:B3 A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12"/>
+  <sheetFormatPr defaultColWidth="11.35546875" defaultRowHeight="12" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.3418367346939"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="22.1"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4692,10 +4684,20 @@
         <v>1357</v>
       </c>
     </row>
+    <row r="4" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>1358</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>1359</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.789583333333333" right="0.789583333333333" top="1.01944444444444" bottom="1.01944444444444" header="0.789583333333333" footer="0.789583333333333"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPágina &amp;P</oddFooter>
@@ -4704,50 +4706,43 @@
 </file>
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:A5"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1:B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12"/>
+  <sheetFormatPr defaultColWidth="11.35546875" defaultRowHeight="12" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.3418367346939"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="60.12"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
         <v>1355</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B1" s="3"/>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
         <v>1356</v>
       </c>
-    </row>
-    <row r="3" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B2" s="3"/>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>1358</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
-        <v>1359</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
         <v>1360</v>
       </c>
+      <c r="B3" s="3"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.789583333333333" right="0.789583333333333" top="1.01944444444444" bottom="1.01944444444444" header="0.789583333333333" footer="0.789583333333333"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPágina &amp;P</oddFooter>
@@ -4756,20 +4751,19 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:A246"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A40" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A45" activeCellId="0" sqref="A45"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A40" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A45" activeCellId="1" sqref="B1:B3 A45"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12"/>
+  <sheetFormatPr defaultColWidth="11.35546875" defaultRowHeight="12" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="24.9744897959184"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="11.3418367346939"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="24.97"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6005,7 +5999,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.789583333333333" right="0.789583333333333" top="1.01944444444444" bottom="1.01944444444444" header="0.789583333333333" footer="0.789583333333333"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPágina &amp;P</oddFooter>
@@ -6014,20 +6008,19 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:A33"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A31" activeCellId="0" sqref="A31"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A31" activeCellId="1" sqref="B1:B3 A31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12"/>
+  <sheetFormatPr defaultColWidth="11.35546875" defaultRowHeight="12" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.6785714285714"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="11.3418367346939"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="22.68"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6198,7 +6191,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.789583333333333" right="0.789583333333333" top="1.01944444444444" bottom="1.01944444444444" header="0.789583333333333" footer="0.789583333333333"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPágina &amp;P</oddFooter>
@@ -6207,20 +6200,19 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:A1032"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A28" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A28" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B7" activeCellId="1" sqref="B1:B3 B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12"/>
+  <sheetFormatPr defaultColWidth="11.35546875" defaultRowHeight="12" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.8112244897959"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="11.3418367346939"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="22.81"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11386,7 +11378,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.789583333333333" right="0.789583333333333" top="1.01944444444444" bottom="1.01944444444444" header="0.789583333333333" footer="0.789583333333333"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPágina &amp;P</oddFooter>
@@ -11395,24 +11387,21 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="B1:B3 A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.3418367346939"/>
-  </cols>
+  <sheetFormatPr defaultColWidth="11.35546875" defaultRowHeight="12" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.789583333333333" right="0.789583333333333" top="1.01944444444444" bottom="1.01944444444444" header="0.789583333333333" footer="0.789583333333333"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPágina &amp;P</oddFooter>
@@ -11421,24 +11410,21 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="B1:B3 A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.3418367346939"/>
-  </cols>
+  <sheetFormatPr defaultColWidth="11.35546875" defaultRowHeight="12" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.789583333333333" right="0.789583333333333" top="1.01944444444444" bottom="1.01944444444444" header="0.789583333333333" footer="0.789583333333333"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPágina &amp;P</oddFooter>
@@ -11447,20 +11433,19 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:A10"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A15" activeCellId="0" sqref="A15"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A15" activeCellId="1" sqref="B1:B3 A15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12"/>
+  <sheetFormatPr defaultColWidth="11.35546875" defaultRowHeight="12" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="26.5918367346939"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="11.3418367346939"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="26.59"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11516,7 +11501,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.789583333333333" right="0.789583333333333" top="1.01944444444444" bottom="1.01944444444444" header="0.789583333333333" footer="0.789583333333333"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPágina &amp;P</oddFooter>
@@ -11525,20 +11510,17 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:A6"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C10" activeCellId="0" sqref="C10"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C10" activeCellId="1" sqref="B1:B3 C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.3418367346939"/>
-  </cols>
+  <sheetFormatPr defaultColWidth="11.35546875" defaultRowHeight="12" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
@@ -11573,7 +11555,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.789583333333333" right="0.789583333333333" top="1.01944444444444" bottom="1.01944444444444" header="0.789583333333333" footer="0.789583333333333"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPágina &amp;P</oddFooter>
@@ -11582,20 +11564,17 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:A4"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="B1:B3 A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.3418367346939"/>
-  </cols>
+  <sheetFormatPr defaultColWidth="11.35546875" defaultRowHeight="12" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
@@ -11620,7 +11599,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.789583333333333" right="0.789583333333333" top="1.01944444444444" bottom="1.01944444444444" header="0.789583333333333" footer="0.789583333333333"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPágina &amp;P</oddFooter>

</xml_diff>